<commit_message>
Claude simplifies the algorithm
</commit_message>
<xml_diff>
--- a/tests/sample_input_test.xlsx
+++ b/tests/sample_input_test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="108">
   <si>
     <t xml:space="preserve">ДАТА</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">TANK 300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">водитель</t>
   </si>
   <si>
     <t xml:space="preserve">водительский коврик</t>
@@ -628,11 +625,11 @@
   </sheetPr>
   <dimension ref="A1:P265"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.80078125" defaultRowHeight="51" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.80859375" defaultRowHeight="51" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="56.45"/>
@@ -998,7 +995,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>23</v>
@@ -1016,7 +1013,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1028,10 +1025,10 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -1064,10 +1061,10 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -1099,10 +1096,10 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -1110,7 +1107,7 @@
         <v>22</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>24</v>
@@ -1137,15 +1134,15 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="7" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>23</v>
@@ -1163,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1175,10 +1172,10 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1213,10 +1210,10 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1251,10 +1248,10 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -1289,10 +1286,10 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1327,10 +1324,10 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1365,15 +1362,15 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>23</v>
@@ -1403,10 +1400,10 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1441,15 +1438,15 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>23</v>
@@ -1479,15 +1476,15 @@
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>23</v>
@@ -1517,18 +1514,18 @@
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>24</v>
@@ -1555,18 +1552,18 @@
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>24</v>
@@ -1581,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1593,21 +1590,21 @@
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>23</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K26" s="5" t="n">
         <v>11</v>
@@ -1619,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1631,15 +1628,15 @@
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>23</v>
@@ -1657,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1669,18 +1666,18 @@
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>24</v>
@@ -1695,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1707,18 +1704,18 @@
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>24</v>
@@ -1733,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1745,18 +1742,18 @@
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>24</v>
@@ -1783,18 +1780,18 @@
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>24</v>
@@ -1809,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1821,18 +1818,18 @@
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>24</v>
@@ -1859,15 +1856,15 @@
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>23</v>
@@ -1897,18 +1894,18 @@
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>24</v>
@@ -1935,18 +1932,18 @@
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>24</v>
@@ -1961,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1973,18 +1970,18 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>24</v>
@@ -2011,15 +2008,15 @@
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>23</v>
@@ -2049,18 +2046,18 @@
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>24</v>
@@ -2087,10 +2084,10 @@
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>

</xml_diff>

<commit_message>
Add test & UI fix
</commit_message>
<xml_diff>
--- a/tests/sample_input_test.xlsx
+++ b/tests/sample_input_test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="111">
   <si>
     <t xml:space="preserve">ДАТА</t>
   </si>
@@ -91,6 +91,9 @@
     <t xml:space="preserve">SSANG YONG ACTYON 2</t>
   </si>
   <si>
+    <t xml:space="preserve">ЯМ</t>
+  </si>
+  <si>
     <t xml:space="preserve">борт</t>
   </si>
   <si>
@@ -202,10 +205,16 @@
     <t xml:space="preserve">VOLKSWAGEN TIGUAN 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Озон</t>
+  </si>
+  <si>
     <t xml:space="preserve">EVA_BORT+Volkswagen+_Tiguan+2016-2021+black+12</t>
   </si>
   <si>
     <t xml:space="preserve">VOLKSWAGEN TIGUAN 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ВБ</t>
   </si>
   <si>
     <t xml:space="preserve">PERED_EVA_Volkswagen_Touareg_I пок и R_2002-2010_black+12</t>
@@ -485,7 +494,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,6 +516,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -625,11 +638,11 @@
   </sheetPr>
   <dimension ref="A1:P265"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.80859375" defaultRowHeight="51" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.81640625" defaultRowHeight="51" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="56.45"/>
@@ -728,16 +741,18 @@
       <c r="E3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="5" t="n">
         <v>12</v>
@@ -761,21 +776,23 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>12</v>
@@ -799,21 +816,23 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>12</v>
@@ -837,21 +856,23 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K6" s="5" t="n">
         <v>12</v>
@@ -875,21 +896,23 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>12</v>
@@ -901,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -913,21 +936,23 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>12</v>
@@ -943,65 +968,69 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="A9" s="7" t="n">
+        <v>45880</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>45880</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7" t="s">
+      <c r="E9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="I9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="J9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="L9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" s="7"/>
+      <c r="L9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="A10" s="7" t="n">
+        <v>45880</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>45880</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>12</v>
@@ -1013,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1024,131 +1053,139 @@
         <v>45880</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7" t="s">
+      <c r="E11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="G11" s="8"/>
+      <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="I11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="7" t="n">
+      <c r="J11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="L11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" s="7"/>
+      <c r="L11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="n">
+      <c r="A12" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7" t="s">
+      <c r="E12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="I12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="7" t="n">
+      <c r="J12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="L12" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" s="7" t="n">
+      <c r="L12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
+      <c r="A13" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7" t="s">
+      <c r="E13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="7" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="8" t="n">
+        <v>11</v>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="n">
+        <v>45870</v>
+      </c>
+      <c r="B14" s="9" t="n">
+        <v>45871</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="7" t="n">
-        <v>11</v>
-      </c>
-      <c r="L13" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M13" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B14" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="J14" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K14" s="5" t="n">
         <v>15</v>
@@ -1159,34 +1196,36 @@
       <c r="M14" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="N14" s="7" t="s">
-        <v>50</v>
+      <c r="N14" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="n">
+      <c r="A15" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="E15" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K15" s="5" t="n">
         <v>11</v>
@@ -1202,105 +1241,111 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="n">
+      <c r="A16" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B16" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="B16" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7" t="s">
+      <c r="E16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="I16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="7" t="n">
+      <c r="J16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="L16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" s="7" t="n">
+      <c r="L16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B17" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="A17" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B17" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7" t="s">
+      <c r="E17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="I17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="7" t="n">
+      <c r="J17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="L17" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N17" s="7" t="n">
+      <c r="L17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B18" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C18" s="8"/>
+      <c r="A18" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B18" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C18" s="9"/>
       <c r="D18" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K18" s="5" t="n">
         <v>12</v>
@@ -1316,29 +1361,31 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="n">
+      <c r="A19" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K19" s="5" t="n">
         <v>12</v>
@@ -1354,67 +1401,71 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="n">
+      <c r="A20" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B20" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="I20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="7" t="n">
+      <c r="J20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="L20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N20" s="7" t="n">
+      <c r="L20" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="n">
+      <c r="A21" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B21" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K21" s="5" t="n">
         <v>12</v>
@@ -1430,29 +1481,31 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="n">
+      <c r="A22" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B22" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="5"/>
+      <c r="B22" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K22" s="5" t="n">
         <v>2</v>
@@ -1468,29 +1521,31 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="n">
+      <c r="A23" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B23" s="8" t="n">
+      <c r="B23" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K23" s="5" t="n">
         <v>2</v>
@@ -1506,29 +1561,31 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B24" s="8" t="n">
+      <c r="A24" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B24" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K24" s="5" t="n">
         <v>11</v>
@@ -1544,29 +1601,31 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B25" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C25" s="8"/>
+      <c r="A25" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B25" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C25" s="9"/>
       <c r="D25" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K25" s="5" t="n">
         <v>11</v>
@@ -1578,33 +1637,35 @@
         <v>0</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="n">
+      <c r="A26" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="B26" s="8" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C26" s="8"/>
+      <c r="B26" s="9" t="n">
+        <v>45880</v>
+      </c>
+      <c r="C26" s="9"/>
       <c r="D26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K26" s="5" t="n">
         <v>11</v>
@@ -1616,33 +1677,35 @@
         <v>0</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B27" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C27" s="8"/>
+      <c r="A27" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B27" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C27" s="9"/>
       <c r="D27" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K27" s="5" t="n">
         <v>13</v>
@@ -1654,71 +1717,75 @@
         <v>0</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B28" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K28" s="7" t="n">
+      <c r="A28" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B28" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="L28" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="7" t="s">
-        <v>83</v>
+      <c r="L28" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="n">
+      <c r="A29" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K29" s="5" t="n">
         <v>11</v>
@@ -1730,33 +1797,35 @@
         <v>0</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="n">
+      <c r="A30" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B30" s="8" t="n">
+      <c r="B30" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C30" s="8"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K30" s="5" t="n">
         <v>11</v>
@@ -1772,29 +1841,31 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B31" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C31" s="8"/>
+      <c r="A31" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B31" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C31" s="9"/>
       <c r="D31" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K31" s="5" t="n">
         <v>11</v>
@@ -1806,33 +1877,35 @@
         <v>0</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B32" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C32" s="8"/>
+      <c r="A32" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B32" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C32" s="9"/>
       <c r="D32" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K32" s="5" t="n">
         <v>11</v>
@@ -1848,29 +1921,31 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B33" s="8" t="n">
+      <c r="A33" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B33" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C33" s="8"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K33" s="5" t="n">
         <v>11</v>
@@ -1886,29 +1961,31 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="n">
+      <c r="A34" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B34" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C34" s="8"/>
+      <c r="B34" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C34" s="9"/>
       <c r="D34" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K34" s="5" t="n">
         <v>8</v>
@@ -1924,29 +2001,31 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B35" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C35" s="8"/>
+      <c r="A35" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B35" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C35" s="9"/>
       <c r="D35" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K35" s="5" t="n">
         <v>11</v>
@@ -1958,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1970,21 +2049,23 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K36" s="5" t="n">
         <v>12</v>
@@ -2008,21 +2089,23 @@
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K37" s="5" t="n">
         <v>2</v>
@@ -2038,29 +2121,31 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="n">
+      <c r="A38" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="B38" s="8" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C38" s="8"/>
+      <c r="B38" s="9" t="n">
+        <v>45880</v>
+      </c>
+      <c r="C38" s="9"/>
       <c r="D38" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>108</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G38" s="5"/>
       <c r="H38" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K38" s="5" t="n">
         <v>11</v>
@@ -2076,29 +2161,31 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8" t="n">
+      <c r="A39" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B39" s="8" t="n">
+      <c r="B39" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C39" s="8"/>
+      <c r="C39" s="9"/>
       <c r="D39" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>110</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="G39" s="5"/>
       <c r="H39" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K39" s="5" t="n">
         <v>11</v>
@@ -2114,94 +2201,94 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="n">
+      <c r="A40" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B40" s="8" t="n">
+      <c r="B40" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C40" s="8"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="n">
+      <c r="A41" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B41" s="8" t="n">
+      <c r="B41" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C41" s="8"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="n">
+      <c r="A42" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B42" s="8" t="n">
+      <c r="B42" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C42" s="8"/>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="n">
+      <c r="A43" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B43" s="8" t="n">
+      <c r="B43" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C43" s="8"/>
+      <c r="C43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="n">
+      <c r="A44" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B44" s="8" t="n">
+      <c r="B44" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C44" s="8"/>
+      <c r="C44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B45" s="8" t="n">
+      <c r="A45" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B45" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C45" s="8"/>
+      <c r="C45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B46" s="8" t="n">
+      <c r="A46" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B46" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C46" s="8"/>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B47" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C47" s="8"/>
+      <c r="A47" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B47" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="n">
+      <c r="A48" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B48" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C48" s="8"/>
+      <c r="B48" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B49" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C49" s="8"/>
+      <c r="A49" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B49" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="n">
@@ -2213,67 +2300,67 @@
       <c r="C50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="n">
+      <c r="A51" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B51" s="8" t="n">
+      <c r="B51" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C51" s="8"/>
+      <c r="C51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="n">
+      <c r="A52" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B52" s="8" t="n">
+      <c r="B52" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C52" s="8"/>
+      <c r="C52" s="9"/>
     </row>
     <row r="53" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="n">
+      <c r="A53" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B53" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C53" s="8"/>
+      <c r="B53" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="n">
+      <c r="A54" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B54" s="8" t="n">
+      <c r="B54" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C54" s="8"/>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B55" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C55" s="8"/>
+      <c r="A55" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B55" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8" t="n">
+      <c r="A56" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="B56" s="8" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C56" s="8"/>
+      <c r="B56" s="9" t="n">
+        <v>45880</v>
+      </c>
+      <c r="C56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="n">
+      <c r="A57" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B57" s="8" t="n">
+      <c r="B57" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C57" s="8"/>
+      <c r="C57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="n">
@@ -2294,31 +2381,31 @@
       <c r="C59" s="4"/>
     </row>
     <row r="60" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="n">
+      <c r="A60" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B60" s="8" t="n">
+      <c r="B60" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C60" s="8"/>
+      <c r="C60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="13" t="n">
+      <c r="A61" s="14" t="n">
         <v>45869</v>
       </c>
-      <c r="B61" s="13" t="n">
+      <c r="B61" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C61" s="13"/>
+      <c r="C61" s="14"/>
     </row>
     <row r="62" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="n">
+      <c r="A62" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B62" s="8" t="n">
+      <c r="B62" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C62" s="8"/>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="n">
@@ -2330,85 +2417,85 @@
       <c r="C63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B64" s="8" t="n">
+      <c r="A64" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B64" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C64" s="8"/>
+      <c r="C64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="n">
+      <c r="A65" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B65" s="8" t="n">
+      <c r="B65" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C65" s="8"/>
+      <c r="C65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8" t="n">
+      <c r="A66" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B66" s="8" t="n">
+      <c r="B66" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C66" s="8"/>
+      <c r="C66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8" t="n">
+      <c r="A67" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B67" s="8" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C67" s="8"/>
+      <c r="B67" s="9" t="n">
+        <v>45880</v>
+      </c>
+      <c r="C67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B68" s="8" t="n">
+      <c r="A68" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B68" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C68" s="8"/>
+      <c r="C68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="13" t="n">
+      <c r="A69" s="14" t="n">
         <v>45869</v>
       </c>
-      <c r="B69" s="13" t="n">
+      <c r="B69" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C69" s="13"/>
+      <c r="C69" s="14"/>
     </row>
     <row r="70" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B70" s="8" t="n">
+      <c r="A70" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B70" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C70" s="8"/>
+      <c r="C70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8" t="n">
+      <c r="A71" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B71" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C71" s="8"/>
+      <c r="B71" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="n">
+      <c r="A72" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B72" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C72" s="8"/>
+      <c r="B72" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C72" s="9"/>
     </row>
     <row r="73" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="n">
@@ -2438,229 +2525,229 @@
       <c r="C75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8" t="n">
+      <c r="A76" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B76" s="8" t="n">
+      <c r="B76" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C76" s="8"/>
+      <c r="C76" s="9"/>
     </row>
     <row r="77" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8" t="n">
+      <c r="A77" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B77" s="8" t="n">
+      <c r="B77" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C77" s="8"/>
+      <c r="C77" s="9"/>
     </row>
     <row r="78" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B78" s="8" t="n">
+      <c r="A78" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B78" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C78" s="8"/>
+      <c r="C78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B79" s="8" t="n">
+      <c r="A79" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B79" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C79" s="8"/>
+      <c r="C79" s="9"/>
     </row>
     <row r="80" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B80" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C80" s="8"/>
+      <c r="A80" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B80" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B81" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C81" s="8"/>
+      <c r="A81" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B81" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C81" s="9"/>
     </row>
     <row r="82" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B82" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C82" s="8"/>
+      <c r="A82" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B82" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="n">
+      <c r="A83" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B83" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C83" s="8"/>
+      <c r="B83" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C83" s="9"/>
     </row>
     <row r="84" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="8" t="n">
+      <c r="A84" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B84" s="8" t="n">
+      <c r="B84" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C84" s="8"/>
+      <c r="C84" s="9"/>
     </row>
     <row r="85" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="8" t="n">
+      <c r="A85" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B85" s="8" t="n">
+      <c r="B85" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C85" s="8"/>
+      <c r="C85" s="9"/>
     </row>
     <row r="86" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="8" t="n">
+      <c r="A86" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B86" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C86" s="8"/>
+      <c r="B86" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="8" t="n">
+      <c r="A87" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B87" s="8" t="n">
+      <c r="B87" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C87" s="8"/>
+      <c r="C87" s="9"/>
     </row>
     <row r="88" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="8" t="n">
+      <c r="A88" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B88" s="8" t="n">
+      <c r="B88" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C88" s="8"/>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B89" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C89" s="8"/>
+      <c r="A89" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B89" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C89" s="9"/>
     </row>
     <row r="90" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="8" t="n">
+      <c r="A90" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B90" s="8" t="n">
+      <c r="B90" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C90" s="8"/>
+      <c r="C90" s="9"/>
     </row>
     <row r="91" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B91" s="8" t="n">
+      <c r="A91" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B91" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C91" s="8"/>
+      <c r="C91" s="9"/>
     </row>
     <row r="92" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B92" s="8" t="n">
+      <c r="A92" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B92" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C92" s="8"/>
+      <c r="C92" s="9"/>
     </row>
     <row r="93" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B93" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C93" s="8"/>
+      <c r="A93" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B93" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C93" s="9"/>
     </row>
     <row r="94" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B94" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C94" s="8"/>
+      <c r="A94" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B94" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C94" s="9"/>
     </row>
     <row r="95" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="8" t="n">
+      <c r="A95" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B95" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C95" s="8"/>
+      <c r="B95" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C95" s="9"/>
     </row>
     <row r="96" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="8" t="n">
+      <c r="A96" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B96" s="8" t="n">
+      <c r="B96" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C96" s="8"/>
+      <c r="C96" s="9"/>
     </row>
     <row r="97" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="8" t="n">
+      <c r="A97" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B97" s="8" t="n">
+      <c r="B97" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C97" s="8"/>
+      <c r="C97" s="9"/>
     </row>
     <row r="98" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B98" s="8" t="n">
+      <c r="A98" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B98" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C98" s="8"/>
+      <c r="C98" s="9"/>
     </row>
     <row r="99" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B99" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C99" s="8"/>
+      <c r="A99" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B99" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C99" s="9"/>
     </row>
     <row r="100" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="8" t="n">
+      <c r="A100" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B100" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C100" s="8"/>
+      <c r="B100" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="n">
@@ -2672,85 +2759,85 @@
       <c r="C101" s="4"/>
     </row>
     <row r="102" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="8" t="n">
+      <c r="A102" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B102" s="8" t="n">
+      <c r="B102" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C102" s="8"/>
+      <c r="C102" s="9"/>
     </row>
     <row r="103" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B103" s="8" t="n">
+      <c r="A103" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B103" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C103" s="8"/>
+      <c r="C103" s="9"/>
     </row>
     <row r="104" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="8" t="n">
+      <c r="A104" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B104" s="8" t="n">
+      <c r="B104" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C104" s="8"/>
+      <c r="C104" s="9"/>
     </row>
     <row r="105" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="8" t="n">
+      <c r="A105" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B105" s="8" t="n">
+      <c r="B105" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C105" s="8"/>
+      <c r="C105" s="9"/>
     </row>
     <row r="106" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="8" t="n">
+      <c r="A106" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B106" s="8" t="n">
+      <c r="B106" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C106" s="8"/>
+      <c r="C106" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B107" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C107" s="8"/>
+      <c r="A107" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B107" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B108" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C108" s="8"/>
+      <c r="A108" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B108" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B109" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C109" s="8"/>
+      <c r="A109" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B109" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B110" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C110" s="8"/>
+      <c r="A110" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B110" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="n">
@@ -2762,121 +2849,121 @@
       <c r="C111" s="4"/>
     </row>
     <row r="112" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="8" t="n">
+      <c r="A112" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B112" s="8" t="n">
+      <c r="B112" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C112" s="8"/>
+      <c r="C112" s="9"/>
     </row>
     <row r="113" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="8" t="n">
+      <c r="A113" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B113" s="8" t="n">
+      <c r="B113" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C113" s="8"/>
+      <c r="C113" s="9"/>
     </row>
     <row r="114" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="8" t="n">
+      <c r="A114" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B114" s="8" t="n">
+      <c r="B114" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C114" s="8"/>
+      <c r="C114" s="9"/>
     </row>
     <row r="115" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="8" t="n">
+      <c r="A115" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B115" s="8" t="n">
+      <c r="B115" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C115" s="8"/>
+      <c r="C115" s="9"/>
     </row>
     <row r="116" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B116" s="8" t="n">
+      <c r="A116" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B116" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C116" s="8"/>
+      <c r="C116" s="9"/>
     </row>
     <row r="117" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="8" t="n">
+      <c r="A117" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B117" s="8" t="n">
+      <c r="B117" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C117" s="8"/>
+      <c r="C117" s="9"/>
     </row>
     <row r="118" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B118" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C118" s="8"/>
+      <c r="A118" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B118" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C118" s="9"/>
     </row>
     <row r="119" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B119" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C119" s="8"/>
+      <c r="A119" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B119" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C119" s="9"/>
     </row>
     <row r="120" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="13" t="n">
+      <c r="A120" s="14" t="n">
         <v>45869</v>
       </c>
-      <c r="B120" s="13" t="n">
+      <c r="B120" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C120" s="13"/>
+      <c r="C120" s="14"/>
     </row>
     <row r="121" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="8" t="n">
+      <c r="A121" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B121" s="8" t="n">
+      <c r="B121" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C121" s="8"/>
+      <c r="C121" s="9"/>
     </row>
     <row r="122" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B122" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C122" s="8"/>
+      <c r="A122" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B122" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C122" s="9"/>
     </row>
     <row r="123" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="8" t="n">
+      <c r="A123" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B123" s="8" t="n">
+      <c r="B123" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C123" s="8"/>
+      <c r="C123" s="9"/>
     </row>
     <row r="124" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B124" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C124" s="8"/>
+      <c r="A124" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B124" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C124" s="9"/>
     </row>
     <row r="125" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="n">
@@ -2888,625 +2975,625 @@
       <c r="C125" s="4"/>
     </row>
     <row r="126" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="8" t="n">
+      <c r="A126" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="B126" s="8" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C126" s="8"/>
+      <c r="B126" s="9" t="n">
+        <v>45880</v>
+      </c>
+      <c r="C126" s="9"/>
     </row>
     <row r="127" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="8" t="n">
+      <c r="A127" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="B127" s="8" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C127" s="8"/>
+      <c r="B127" s="9" t="n">
+        <v>45880</v>
+      </c>
+      <c r="C127" s="9"/>
     </row>
     <row r="128" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="8" t="n">
+      <c r="A128" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B128" s="8" t="n">
+      <c r="B128" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C128" s="8"/>
+      <c r="C128" s="9"/>
     </row>
     <row r="129" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="8" t="n">
+      <c r="A129" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B129" s="8" t="n">
+      <c r="B129" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C129" s="8"/>
+      <c r="C129" s="9"/>
     </row>
     <row r="130" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="8" t="n">
+      <c r="A130" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B130" s="8" t="n">
+      <c r="B130" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C130" s="8"/>
+      <c r="C130" s="9"/>
     </row>
     <row r="131" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="8" t="n">
+      <c r="A131" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B131" s="8" t="n">
+      <c r="B131" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C131" s="8"/>
+      <c r="C131" s="9"/>
     </row>
     <row r="132" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B132" s="8" t="n">
+      <c r="A132" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B132" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C132" s="8"/>
+      <c r="C132" s="9"/>
     </row>
     <row r="133" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B133" s="8" t="n">
+      <c r="A133" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B133" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C133" s="8"/>
+      <c r="C133" s="9"/>
     </row>
     <row r="134" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B134" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C134" s="8"/>
+      <c r="A134" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B134" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C134" s="9"/>
     </row>
     <row r="135" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B135" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C135" s="8"/>
+      <c r="A135" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B135" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C135" s="9"/>
     </row>
     <row r="136" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B136" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C136" s="8"/>
+      <c r="A136" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B136" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C136" s="9"/>
     </row>
     <row r="137" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B137" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C137" s="8"/>
+      <c r="A137" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B137" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C137" s="9"/>
     </row>
     <row r="138" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B138" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C138" s="8"/>
+      <c r="A138" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B138" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C138" s="9"/>
     </row>
     <row r="139" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B139" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C139" s="8"/>
+      <c r="A139" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B139" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C139" s="9"/>
     </row>
     <row r="140" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B140" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C140" s="8"/>
+      <c r="A140" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B140" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C140" s="9"/>
     </row>
     <row r="141" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="8" t="n">
+      <c r="A141" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B141" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C141" s="8"/>
+      <c r="B141" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C141" s="9"/>
     </row>
     <row r="142" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="8" t="n">
+      <c r="A142" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B142" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C142" s="8"/>
+      <c r="B142" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C142" s="9"/>
     </row>
     <row r="143" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="8" t="n">
+      <c r="A143" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B143" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C143" s="8"/>
+      <c r="B143" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C143" s="9"/>
     </row>
     <row r="144" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="8" t="n">
+      <c r="A144" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B144" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C144" s="8"/>
+      <c r="B144" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C144" s="9"/>
     </row>
     <row r="145" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="8" t="n">
+      <c r="A145" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B145" s="8" t="n">
+      <c r="B145" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C145" s="8"/>
+      <c r="C145" s="9"/>
     </row>
     <row r="146" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="8" t="n">
+      <c r="A146" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B146" s="8" t="n">
+      <c r="B146" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C146" s="8"/>
+      <c r="C146" s="9"/>
     </row>
     <row r="147" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B147" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C147" s="8"/>
+      <c r="A147" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B147" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C147" s="9"/>
     </row>
     <row r="148" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="8" t="n">
+      <c r="A148" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B148" s="8" t="n">
+      <c r="B148" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C148" s="8"/>
+      <c r="C148" s="9"/>
     </row>
     <row r="149" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B149" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C149" s="8"/>
+      <c r="A149" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B149" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C149" s="9"/>
     </row>
     <row r="150" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="8" t="n">
+      <c r="A150" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B150" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C150" s="8"/>
+      <c r="B150" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C150" s="9"/>
     </row>
     <row r="151" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="8" t="n">
+      <c r="A151" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B151" s="8" t="n">
+      <c r="B151" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C151" s="8"/>
+      <c r="C151" s="9"/>
     </row>
     <row r="152" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="8" t="n">
+      <c r="A152" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B152" s="8" t="n">
+      <c r="B152" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="C152" s="8"/>
+      <c r="C152" s="9"/>
     </row>
     <row r="153" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="8" t="n">
+      <c r="A153" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B153" s="8" t="n">
+      <c r="B153" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C153" s="8"/>
+      <c r="C153" s="9"/>
     </row>
     <row r="154" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A154" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B154" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C154" s="8"/>
+      <c r="A154" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B154" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C154" s="9"/>
     </row>
     <row r="155" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="13" t="n">
+      <c r="A155" s="14" t="n">
         <v>45869</v>
       </c>
-      <c r="B155" s="13" t="n">
+      <c r="B155" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C155" s="13"/>
+      <c r="C155" s="14"/>
     </row>
     <row r="156" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="13" t="n">
+      <c r="A156" s="14" t="n">
         <v>45869</v>
       </c>
-      <c r="B156" s="13" t="n">
+      <c r="B156" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C156" s="13"/>
+      <c r="C156" s="14"/>
     </row>
     <row r="157" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="13" t="n">
+      <c r="A157" s="14" t="n">
         <v>45868</v>
       </c>
-      <c r="B157" s="13" t="n">
+      <c r="B157" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C157" s="13"/>
+      <c r="C157" s="14"/>
     </row>
     <row r="158" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B158" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C158" s="8"/>
+      <c r="A158" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B158" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C158" s="9"/>
     </row>
     <row r="159" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="8" t="n">
+      <c r="A159" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B159" s="8" t="n">
+      <c r="B159" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C159" s="8"/>
+      <c r="C159" s="9"/>
     </row>
     <row r="160" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B160" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C160" s="8"/>
+      <c r="A160" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B160" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C160" s="9"/>
     </row>
     <row r="161" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B161" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C161" s="8"/>
+      <c r="A161" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B161" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C161" s="9"/>
     </row>
     <row r="162" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B162" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C162" s="8"/>
+      <c r="A162" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B162" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C162" s="9"/>
     </row>
     <row r="163" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="13" t="n">
+      <c r="A163" s="14" t="n">
         <v>45869</v>
       </c>
-      <c r="B163" s="13" t="n">
+      <c r="B163" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C163" s="13"/>
+      <c r="C163" s="14"/>
     </row>
     <row r="164" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B164" s="8" t="n">
+      <c r="A164" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B164" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C164" s="8"/>
+      <c r="C164" s="9"/>
     </row>
     <row r="165" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="8" t="n">
+      <c r="A165" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B165" s="8" t="n">
+      <c r="B165" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C165" s="8"/>
+      <c r="C165" s="9"/>
     </row>
     <row r="166" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A166" s="8" t="n">
+      <c r="A166" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B166" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C166" s="8"/>
+      <c r="B166" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C166" s="9"/>
     </row>
     <row r="167" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A167" s="8" t="n">
+      <c r="A167" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B167" s="8" t="n">
+      <c r="B167" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C167" s="8"/>
+      <c r="C167" s="9"/>
     </row>
     <row r="168" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A168" s="8" t="n">
+      <c r="A168" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B168" s="8" t="n">
+      <c r="B168" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C168" s="8"/>
+      <c r="C168" s="9"/>
     </row>
     <row r="169" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B169" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C169" s="8"/>
+      <c r="A169" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B169" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C169" s="9"/>
     </row>
     <row r="170" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B170" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C170" s="8"/>
+      <c r="A170" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B170" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C170" s="9"/>
     </row>
     <row r="171" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A171" s="8" t="n">
+      <c r="A171" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B171" s="8" t="n">
+      <c r="B171" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="C171" s="8"/>
+      <c r="C171" s="9"/>
     </row>
     <row r="172" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B172" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C172" s="8"/>
+      <c r="A172" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B172" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C172" s="9"/>
     </row>
     <row r="173" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B173" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C173" s="8"/>
+      <c r="A173" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B173" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C173" s="9"/>
     </row>
     <row r="174" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A174" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B174" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C174" s="8"/>
+      <c r="A174" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B174" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C174" s="9"/>
     </row>
     <row r="175" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="8" t="n">
+      <c r="A175" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B175" s="8" t="n">
+      <c r="B175" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C175" s="8"/>
+      <c r="C175" s="9"/>
     </row>
     <row r="176" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="8" t="n">
+      <c r="A176" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B176" s="8" t="n">
+      <c r="B176" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C176" s="8"/>
+      <c r="C176" s="9"/>
     </row>
     <row r="177" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="8" t="n">
+      <c r="A177" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B177" s="8" t="n">
+      <c r="B177" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C177" s="8"/>
+      <c r="C177" s="9"/>
     </row>
     <row r="178" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="8" t="n">
+      <c r="A178" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B178" s="8" t="n">
+      <c r="B178" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C178" s="8"/>
+      <c r="C178" s="9"/>
     </row>
     <row r="179" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B179" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C179" s="8"/>
+      <c r="A179" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B179" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C179" s="9"/>
     </row>
     <row r="180" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B180" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C180" s="8"/>
+      <c r="A180" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B180" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C180" s="9"/>
     </row>
     <row r="181" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B181" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C181" s="8"/>
+      <c r="A181" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B181" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C181" s="9"/>
     </row>
     <row r="182" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="8" t="n">
+      <c r="A182" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B182" s="8" t="n">
+      <c r="B182" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C182" s="8"/>
+      <c r="C182" s="9"/>
     </row>
     <row r="183" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="8" t="n">
+      <c r="A183" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B183" s="8" t="n">
+      <c r="B183" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C183" s="8"/>
+      <c r="C183" s="9"/>
     </row>
     <row r="184" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="8" t="n">
+      <c r="A184" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B184" s="8" t="n">
+      <c r="B184" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C184" s="8"/>
+      <c r="C184" s="9"/>
     </row>
     <row r="185" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="8" t="n">
+      <c r="A185" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B185" s="8" t="n">
+      <c r="B185" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C185" s="8"/>
+      <c r="C185" s="9"/>
     </row>
     <row r="186" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="8" t="n">
+      <c r="A186" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B186" s="8" t="n">
+      <c r="B186" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C186" s="8"/>
+      <c r="C186" s="9"/>
     </row>
     <row r="187" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B187" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C187" s="8"/>
+      <c r="A187" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B187" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C187" s="9"/>
     </row>
     <row r="188" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B188" s="8" t="n">
+      <c r="A188" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B188" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C188" s="8"/>
+      <c r="C188" s="9"/>
     </row>
     <row r="189" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B189" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C189" s="8"/>
+      <c r="A189" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B189" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C189" s="9"/>
     </row>
     <row r="190" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="8" t="n">
+      <c r="A190" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B190" s="8" t="n">
+      <c r="B190" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C190" s="8"/>
+      <c r="C190" s="9"/>
     </row>
     <row r="191" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="8" t="n">
+      <c r="A191" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B191" s="8" t="n">
+      <c r="B191" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="C191" s="8"/>
+      <c r="C191" s="9"/>
     </row>
     <row r="192" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B192" s="8" t="n">
+      <c r="A192" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B192" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C192" s="8"/>
+      <c r="C192" s="9"/>
     </row>
     <row r="193" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A193" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B193" s="8" t="n">
+      <c r="A193" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B193" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C193" s="8"/>
+      <c r="C193" s="9"/>
     </row>
     <row r="194" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="8" t="n">
+      <c r="A194" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B194" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C194" s="8"/>
+      <c r="B194" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C194" s="9"/>
     </row>
     <row r="195" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="4" t="n">
@@ -3518,49 +3605,49 @@
       <c r="C195" s="4"/>
     </row>
     <row r="196" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A196" s="8" t="n">
+      <c r="A196" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B196" s="8" t="n">
+      <c r="B196" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C196" s="8"/>
+      <c r="C196" s="9"/>
     </row>
     <row r="197" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A197" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B197" s="8" t="n">
+      <c r="A197" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B197" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C197" s="8"/>
+      <c r="C197" s="9"/>
     </row>
     <row r="198" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A198" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B198" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C198" s="8"/>
+      <c r="A198" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B198" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C198" s="9"/>
     </row>
     <row r="199" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A199" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B199" s="8" t="n">
+      <c r="A199" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B199" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C199" s="8"/>
+      <c r="C199" s="9"/>
     </row>
     <row r="200" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A200" s="8" t="n">
+      <c r="A200" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B200" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C200" s="8"/>
+      <c r="B200" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C200" s="9"/>
     </row>
     <row r="201" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="4" t="n">
@@ -3572,67 +3659,67 @@
       <c r="C201" s="4"/>
     </row>
     <row r="202" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A202" s="8" t="n">
+      <c r="A202" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B202" s="8" t="n">
+      <c r="B202" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C202" s="8"/>
+      <c r="C202" s="9"/>
     </row>
     <row r="203" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A203" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B203" s="8" t="n">
+      <c r="A203" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B203" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="C203" s="8"/>
+      <c r="C203" s="9"/>
     </row>
     <row r="204" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A204" s="8" t="n">
+      <c r="A204" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B204" s="8" t="n">
+      <c r="B204" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C204" s="8"/>
+      <c r="C204" s="9"/>
     </row>
     <row r="205" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A205" s="13" t="n">
+      <c r="A205" s="14" t="n">
         <v>45869</v>
       </c>
-      <c r="B205" s="13" t="n">
+      <c r="B205" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C205" s="13"/>
+      <c r="C205" s="14"/>
     </row>
     <row r="206" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A206" s="13" t="n">
+      <c r="A206" s="14" t="n">
         <v>45869</v>
       </c>
-      <c r="B206" s="13" t="n">
+      <c r="B206" s="14" t="n">
         <v>45870</v>
       </c>
-      <c r="C206" s="13"/>
+      <c r="C206" s="14"/>
     </row>
     <row r="207" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="8" t="n">
+      <c r="A207" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B207" s="8" t="n">
+      <c r="B207" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C207" s="8"/>
+      <c r="C207" s="9"/>
     </row>
     <row r="208" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B208" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C208" s="8"/>
+      <c r="A208" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="B208" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C208" s="9"/>
     </row>
     <row r="209" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="4" t="n">
@@ -3644,67 +3731,67 @@
       <c r="C209" s="4"/>
     </row>
     <row r="210" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A210" s="8" t="n">
+      <c r="A210" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="B210" s="8" t="n">
+      <c r="B210" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C210" s="8"/>
+      <c r="C210" s="9"/>
     </row>
     <row r="211" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A211" s="8" t="n">
+      <c r="A211" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B211" s="8" t="n">
+      <c r="B211" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C211" s="8"/>
+      <c r="C211" s="9"/>
     </row>
     <row r="212" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A212" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B212" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C212" s="8"/>
+      <c r="A212" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="B212" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="C212" s="9"/>
     </row>
     <row r="213" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A213" s="8" t="n">
+      <c r="A213" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B213" s="8" t="n">
+      <c r="B213" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C213" s="8"/>
+      <c r="C213" s="9"/>
     </row>
     <row r="214" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A214" s="8" t="n">
+      <c r="A214" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B214" s="8" t="n">
+      <c r="B214" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C214" s="8"/>
+      <c r="C214" s="9"/>
     </row>
     <row r="215" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A215" s="8" t="n">
+      <c r="A215" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B215" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C215" s="8"/>
+      <c r="B215" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C215" s="9"/>
     </row>
     <row r="216" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A216" s="8" t="n">
+      <c r="A216" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B216" s="8" t="n">
+      <c r="B216" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C216" s="8"/>
+      <c r="C216" s="9"/>
     </row>
     <row r="217" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="4" t="n">
@@ -3725,67 +3812,67 @@
       <c r="C218" s="4"/>
     </row>
     <row r="219" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A219" s="8" t="n">
+      <c r="A219" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="B219" s="8" t="n">
+      <c r="B219" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="C219" s="8"/>
+      <c r="C219" s="9"/>
     </row>
     <row r="220" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A220" s="8" t="n">
+      <c r="A220" s="9" t="n">
         <v>45875</v>
       </c>
-      <c r="B220" s="8" t="n">
+      <c r="B220" s="9" t="n">
         <v>45876</v>
       </c>
-      <c r="C220" s="8"/>
+      <c r="C220" s="9"/>
     </row>
     <row r="221" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A221" s="8" t="n">
+      <c r="A221" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B221" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C221" s="8"/>
+      <c r="B221" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C221" s="9"/>
     </row>
     <row r="222" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A222" s="8" t="n">
+      <c r="A222" s="9" t="n">
         <v>45877</v>
       </c>
-      <c r="B222" s="8" t="n">
+      <c r="B222" s="9" t="n">
         <v>45878</v>
       </c>
-      <c r="C222" s="8"/>
+      <c r="C222" s="9"/>
     </row>
     <row r="223" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A223" s="8" t="n">
+      <c r="A223" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="B223" s="8" t="n">
+      <c r="B223" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="C223" s="8"/>
+      <c r="C223" s="9"/>
     </row>
     <row r="224" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A224" s="8" t="n">
+      <c r="A224" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="B224" s="8" t="n">
+      <c r="B224" s="9" t="n">
         <v>45879</v>
       </c>
-      <c r="C224" s="8"/>
+      <c r="C224" s="9"/>
     </row>
     <row r="225" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A225" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B225" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C225" s="8"/>
+      <c r="A225" s="9" t="n">
+        <v>45873</v>
+      </c>
+      <c r="B225" s="9" t="n">
+        <v>45874</v>
+      </c>
+      <c r="C225" s="9"/>
     </row>
     <row r="226" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="4" t="n">
@@ -3797,13 +3884,13 @@
       <c r="C226" s="4"/>
     </row>
     <row r="227" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A227" s="8" t="n">
+      <c r="A227" s="9" t="n">
         <v>45871</v>
       </c>
-      <c r="B227" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C227" s="8"/>
+      <c r="B227" s="9" t="n">
+        <v>45872</v>
+      </c>
+      <c r="C227" s="9"/>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>